<commit_message>
updated demo data and scripts
</commit_message>
<xml_diff>
--- a/protected/data/excel/issue.xlsx
+++ b/protected/data/excel/issue.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,9 +15,74 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>corrective_action</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>create_time</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>IR00001</t>
+  </si>
+  <si>
+    <t>IR00002</t>
+  </si>
+  <si>
+    <t>P09-001</t>
+  </si>
+  <si>
+    <t>CLOSED</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Connectivity of PCB-type inductor in layout is incorrect.</t>
+  </si>
+  <si>
+    <t>Incorrect PCB layout</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Difficult assembly procedure</t>
+  </si>
+  <si>
+    <t>ASSY</t>
+  </si>
+  <si>
+    <t>Difficult to assemble and test PCA due to copper-side-up orientation. Orienting PCA component-side up allows for full access to components for debugging after assembly.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,14 +111,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +417,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2">
+        <v>38362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2">
+        <v>38407</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>